<commit_message>
xlsx data to db
</commit_message>
<xml_diff>
--- a/user/sample.xlsx
+++ b/user/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -39,7 +39,7 @@
     <t>01316401520</t>
   </si>
   <si>
-    <t>IT</t>
+    <t>B.Tech IT</t>
   </si>
   <si>
     <t>Vishesh Gupta</t>
@@ -51,7 +51,7 @@
     <t>06116401520</t>
   </si>
   <si>
-    <t>CSE</t>
+    <t>B.Tech CSE</t>
   </si>
   <si>
     <t>Nidhi Rathore</t>
@@ -61,13 +61,16 @@
   </si>
   <si>
     <t>03816401520</t>
+  </si>
+  <si>
+    <t>MCA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -78,13 +81,23 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,8 +122,8 @@
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -361,7 +374,7 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -389,8 +402,8 @@
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>